<commit_message>
Create API + DB
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\Code\AudaciaBall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABF614D-6BDD-41F1-900C-B81E0BC1E3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42893167-1B3C-4B5D-94D3-92FB1A0BCB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{7AB96B2F-2B38-4B92-B705-BE7A112521B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Used" sheetId="2" r:id="rId2"/>
+    <sheet name="ToDo API" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>AudaciaBall</t>
   </si>
@@ -68,9 +70,6 @@
     <t>Install node.js (vue)</t>
   </si>
   <si>
-    <t>Install PostgreSQL</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
@@ -80,12 +79,6 @@
     <t>Dev</t>
   </si>
   <si>
-    <t>Create UI with Vue.JS in Visual Studio</t>
-  </si>
-  <si>
-    <t>Create DB with PostgreSQL</t>
-  </si>
-  <si>
     <t>Create API in C# with Visual Studio</t>
   </si>
   <si>
@@ -120,6 +113,60 @@
   </si>
   <si>
     <t>Time it took (hours)</t>
+  </si>
+  <si>
+    <t>Create project + empty DB (Visual Studio)</t>
+  </si>
+  <si>
+    <t>vue-router</t>
+  </si>
+  <si>
+    <t>installed with npm</t>
+  </si>
+  <si>
+    <t>vue-cli</t>
+  </si>
+  <si>
+    <t>Create UI routes with Vue.JS in Visual Studio</t>
+  </si>
+  <si>
+    <t>Add UI components</t>
+  </si>
+  <si>
+    <t>AddTeam</t>
+  </si>
+  <si>
+    <t>AddPlayer</t>
+  </si>
+  <si>
+    <t>AddGame</t>
+  </si>
+  <si>
+    <t>GetGameHistory</t>
+  </si>
+  <si>
+    <t>What</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>string name, int player1, int player2</t>
+  </si>
+  <si>
+    <t>string name</t>
+  </si>
+  <si>
+    <t>int player1, int player2, int scoreBlue, int scoreRed, date date</t>
+  </si>
+  <si>
+    <t>int idPlayer</t>
+  </si>
+  <si>
+    <t>GetScoreboard</t>
+  </si>
+  <si>
+    <t>Create DB SQL Server</t>
   </si>
 </sst>
 </file>
@@ -194,11 +241,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,272 +560,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64609317-DF29-41BD-B05D-49F3BE0D1E1E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="30.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
-        <f t="shared" ref="A7:A16" si="0">A6+1</f>
+      <c r="A7" s="2">
+        <f t="shared" ref="A7:A17" si="0">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
-        <f t="shared" si="0"/>
+      <c r="A12" s="2">
+        <v>7.1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <f>A11+1</f>
         <v>8</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="3">
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="3">
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="2">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="3">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="3">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E22">
+        <f>SUM(E5:E20)</f>
+        <v>7.3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -788,4 +878,115 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A271660-19C8-4AAD-B4AC-C24887D7E978}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA632A2-C145-4394-A5C5-2C62F8E0F0A9}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
API finish last methods
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\Code\AudaciaBall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42893167-1B3C-4B5D-94D3-92FB1A0BCB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3913383-3F13-49DE-B38C-E0C2986E517B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{7AB96B2F-2B38-4B92-B705-BE7A112521B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planning" sheetId="1" r:id="rId1"/>
     <sheet name="Used" sheetId="2" r:id="rId2"/>
     <sheet name="ToDo API" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>AudaciaBall</t>
   </si>
@@ -163,10 +163,16 @@
     <t>int idPlayer</t>
   </si>
   <si>
-    <t>GetScoreboard</t>
-  </si>
-  <si>
     <t>Create DB SQL Server</t>
+  </si>
+  <si>
+    <t>GetAllGames</t>
+  </si>
+  <si>
+    <t>GetAllPlayers</t>
+  </si>
+  <si>
+    <t>GetAllTeams</t>
   </si>
 </sst>
 </file>
@@ -239,13 +245,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64609317-DF29-41BD-B05D-49F3BE0D1E1E}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -756,7 +763,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>24</v>
@@ -780,7 +787,7 @@
         <v>24</v>
       </c>
       <c r="E14" s="2">
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -867,7 +874,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E22">
         <f>SUM(E5:E20)</f>
-        <v>7.3</v>
+        <v>7.8</v>
       </c>
     </row>
   </sheetData>
@@ -913,10 +920,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA632A2-C145-4394-A5C5-2C62F8E0F0A9}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -965,7 +972,9 @@
       <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
@@ -980,10 +989,30 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
publish API, Add vue components, add CORS to API
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Solioz\Documents\Code\AudaciaBall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3913383-3F13-49DE-B38C-E0C2986E517B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FC3CBE-3BA7-47A4-9AAD-3AC3A68F6243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{7AB96B2F-2B38-4B92-B705-BE7A112521B7}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="ToDo API" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>AudaciaBall</t>
   </si>
@@ -106,9 +107,6 @@
     <t>Deploy</t>
   </si>
   <si>
-    <t>Simply deploiement with Docker</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -173,6 +171,21 @@
   </si>
   <si>
     <t>GetAllTeams</t>
+  </si>
+  <si>
+    <t>Create DB on Azure</t>
+  </si>
+  <si>
+    <t>Deploy API on Azure</t>
+  </si>
+  <si>
+    <t>Cors</t>
+  </si>
+  <si>
+    <t>installed with install-package</t>
+  </si>
+  <si>
+    <t>Deploy UI on web</t>
   </si>
 </sst>
 </file>
@@ -249,10 +262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,37 +580,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64609317-DF29-41BD-B05D-49F3BE0D1E1E}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.796875" customWidth="1"/>
     <col min="3" max="3" width="35.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -613,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -627,7 +640,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
         <v>0.5</v>
@@ -645,7 +658,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
         <v>0.1</v>
@@ -653,7 +666,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <f t="shared" ref="A7:A17" si="0">A6+1</f>
+        <f t="shared" ref="A7:A19" si="0">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -663,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2">
         <v>0.1</v>
@@ -678,10 +691,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
         <v>0.1</v>
@@ -699,7 +712,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -717,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2">
         <v>0.5</v>
@@ -732,10 +745,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -749,10 +762,14 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
@@ -763,10 +780,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2">
         <v>0.5</v>
@@ -784,7 +801,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="2">
         <v>4.5</v>
@@ -801,80 +818,118 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10.1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
+        <f>A15+1</f>
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="2">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E22">
-        <f>SUM(E5:E20)</f>
-        <v>7.8</v>
+      <c r="A22" s="2">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E24">
+        <f>SUM(E5:E22)</f>
+        <v>13.3</v>
       </c>
     </row>
   </sheetData>
@@ -889,28 +944,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A271660-19C8-4AAD-B4AC-C24887D7E978}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -934,10 +997,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -945,73 +1008,73 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
-        <v>44</v>
+      <c r="A7" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>45</v>
+      <c r="A8" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>